<commit_message>
Alle Spalten kursiv markiert
</commit_message>
<xml_diff>
--- a/tabelle_1_main.xlsx
+++ b/tabelle_1_main.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="1599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="1600">
   <si>
     <t>phrasem_id</t>
   </si>
@@ -291,7 +291,7 @@
     <t>Während des Meetings hat er wieder einen Witz aus dem Ärmel geschüttelt, um die Stimmung zu heben.</t>
   </si>
   <si>
-    <t>etw. aus der Hand schütteln; zaubern; etw. aus dem Handgelenk schütteln; zaubern; hat; aus dem Ärmel geschüttelt; aus dem Ärmel schütteln</t>
+    <t>etw. aus der Hand schütteln; zaubern; etw. aus dem Handgelenk schütteln; zaubern; hat; aus dem Ärmel geschüttelt; aus dem Ärmel schütteln; etw. aus der Hand schütteln / zaubern, etw. aus dem Handgelenk schütteln /;  zaubern</t>
   </si>
   <si>
     <t>ph00005</t>
@@ -430,7 +430,7 @@
     <t>Heute war ich schlecht vorbereitet bei der Prüfung, aber ich hoffe, dass mein Lehrer ein Auge zudrückt.</t>
   </si>
   <si>
-    <t>ein Auge; zudrücken; drücke, zu; zudrückt</t>
+    <t>ein Auge; zudrücken; drücke, zu; zudrückt; beide Augen zudrücken</t>
   </si>
   <si>
     <t>ph00009</t>
@@ -544,7 +544,7 @@
     <t>Vor dem Zahnarzttermin hatte ich richtig Schiss.</t>
   </si>
   <si>
-    <t>habe; Bammel; hat; hatte; Schiss</t>
+    <t xml:space="preserve">habe; Bammel; hat; hatte; Schiss; Schiss haben </t>
   </si>
   <si>
     <t>ph00012</t>
@@ -580,7 +580,7 @@
     <t>Die Umweltschützer gehen auf die Barrikaden gegen den Bau der neuen Autobahn.</t>
   </si>
   <si>
-    <t xml:space="preserve">auf die Barrikaden; gehen; gingen; </t>
+    <t xml:space="preserve">auf die Barrikaden; gehen; gingen; Barrikade </t>
   </si>
   <si>
     <t>ph00013</t>
@@ -655,7 +655,7 @@
     <t>Wir haben blau gemacht, weil wir müde waren und uns ausruhen wollten.</t>
   </si>
   <si>
-    <t>blau; machen; mache; hat; gemacht; machst; haben;</t>
+    <t>blau; machen; mache; hat; gemacht; machst; haben; blauen Montag machen; Montag;</t>
   </si>
   <si>
     <t>ph00015</t>
@@ -697,7 +697,7 @@
     <t>Nach der Party war er total blau und konnte kaum laufen.</t>
   </si>
   <si>
-    <t xml:space="preserve">blau; sein; warst; war; </t>
+    <t>blau; sein; warst; war; blau vor den Augen werden</t>
   </si>
   <si>
     <t>ph00016</t>
@@ -772,7 +772,7 @@
     <t>Nach dem schweren Niederlage waren alle Spieler am Boden zerstört.</t>
   </si>
   <si>
-    <t xml:space="preserve">am Boden; zerstört; sein; war; ist; waren; </t>
+    <t>am Boden; zerstört; sein; war; ist; waren; den Boden unter den Füßen verlieren</t>
   </si>
   <si>
     <t>ph00018</t>
@@ -811,7 +811,7 @@
     <t>Obwohl wir aus verschiedenen Abteilungen kommen, sitzen wir bei diesem Projekt im gleichen Boot.</t>
   </si>
   <si>
-    <t xml:space="preserve">im; gleichen; einem; Boot; sitzen; </t>
+    <t>im; gleichen; einem; Boot; sitzen; to be in the same boat;</t>
   </si>
   <si>
     <t>ph00019</t>
@@ -844,7 +844,7 @@
     <t>Du redest ständig um den heißen Brei herum, anstatt einfach zuzugeben, dass du einen Fehler gemacht hast.</t>
   </si>
   <si>
-    <t>um den heißen Brei; reden; redest; herum</t>
+    <t>um den heißen Brei; reden; redest; herum; wie die Katze um den heißen Brei schleichen</t>
   </si>
   <si>
     <t>ph00020</t>
@@ -1015,7 +1015,7 @@
     <t>Auch wenn es schwierig wird, bleibt sie guter Dinge und kämpft weiter.</t>
   </si>
   <si>
-    <t>guter Dinge; sein; ist; bin; bleibt</t>
+    <t>guter Dinge; sein; ist; bin; bleibt; aller guten Dinge sind; gute Dinge sein</t>
   </si>
   <si>
     <t>ph00025</t>
@@ -1459,7 +1459,7 @@
     <t xml:space="preserve">Bist du mit der Präsentation fertig? - Ja, alles im grünen Bereich, ich habe alles gut vorbereitet. </t>
   </si>
   <si>
-    <t xml:space="preserve">alles im grünen Bereich; sein; ist; </t>
+    <t xml:space="preserve">alles im grünen Bereich; sein; ist; Alles in einem grünen Bereich; Alles ist grüner Bereich </t>
   </si>
   <si>
     <t>ph00038</t>
@@ -1498,7 +1498,7 @@
     <t>Ich bekomme immer einen Kloß im Hals, wenn ich an meine Kindheit denke.</t>
   </si>
   <si>
-    <t>einen Kloß im Hals; haben; hatte; bekomme</t>
+    <t xml:space="preserve">einen Kloß im Hals; haben; hatte; bekomme; Knödel; Kloß; Knödeltenor </t>
   </si>
   <si>
     <t>ph00039</t>
@@ -1561,7 +1561,7 @@
     <t>Ich könnte aus der Haut fahren, wenn mein Auto schon wieder kaputt ist.</t>
   </si>
   <si>
-    <t xml:space="preserve">aus der Haut; fahren; bin; gefahren; fährt; </t>
+    <t>aus der Haut; fahren; bin; gefahren; fährt; Nicht aus seiner Haut können</t>
   </si>
   <si>
     <t>ph00041</t>
@@ -1999,7 +1999,7 @@
     <t>Er war lange auf dem Holzweg, bevor er die richtige Lösung fand.</t>
   </si>
   <si>
-    <t xml:space="preserve">auf dem Holzweg; sein; war; bist; ist; </t>
+    <t>auf dem Holzweg; sein; war; bist; ist; "Holzweg";</t>
   </si>
   <si>
     <t>ph00055</t>
@@ -2242,7 +2242,7 @@
     <t>In dem Krimi wollte der Angeklagte eine Zeugin kalt machen.</t>
   </si>
   <si>
-    <t xml:space="preserve">kalt; machen; macht; </t>
+    <t>kalt; machen; macht; “kalt”;</t>
   </si>
   <si>
     <t>ph00062</t>
@@ -2275,7 +2275,7 @@
     <t>Wir dürfen jetzt nicht alle Mitarbeiter über einen Kamm scheren! Wir müssen unterscheiden zwischen denen, die sich um eine Lösung bemüht haben, und denen, die kein Interesse gezeigt haben.</t>
   </si>
   <si>
-    <t xml:space="preserve">über einen Kamm; scheren; </t>
+    <t>über einen Kamm; scheren; Bader;</t>
   </si>
   <si>
     <t>ph00063</t>
@@ -2338,7 +2338,7 @@
     <t>Heute bin ich total verkatert , denn gestern habe ich meinen Geburtstag gefeiert.</t>
   </si>
   <si>
-    <t>einen Kater; haben; hatte; Katers; bin; verkatert</t>
+    <t>einen Kater; haben; hatte; Katers; bin; verkatert; sein</t>
   </si>
   <si>
     <t>ph00065</t>
@@ -2371,7 +2371,7 @@
     <t>Nun lässt die Regierung die Katze aus dem Sack: Energiepreise werden deutlich teurer als bisher angenommen.</t>
   </si>
   <si>
-    <t xml:space="preserve">die Katze aus dem Sack; lassen; ist; los; Katze, lässt; </t>
+    <t>die Katze aus dem Sack; lassen; ist; los; Katze, lässt; die Katze im Sack lassen</t>
   </si>
   <si>
     <t>ph00066</t>
@@ -2464,7 +2464,7 @@
     <t>Deine Diskussionen gehen mir auf die Nerven. Halt einfach mal die Klappe!</t>
   </si>
   <si>
-    <t xml:space="preserve">die Klappe; halten; halt; </t>
+    <t>die Klappe; halten; halt; Klappe;</t>
   </si>
   <si>
     <t>ph00069</t>
@@ -2617,7 +2617,7 @@
     <t>Nach mehreren Dates hat sie ihm schließlich einen Korb gegeben, weil die Chemie einfach nicht stimmte.</t>
   </si>
   <si>
-    <t>einen Korb; geben; haben; gegeben; gibt; hat;</t>
+    <t>einen Korb; geben; haben; gegeben; gibt; hat; bekommen;</t>
   </si>
   <si>
     <t>ph00074</t>
@@ -2710,7 +2710,7 @@
     <t>Ein Betriebsausflug hält die Mitarbeiter bei Laune.</t>
   </si>
   <si>
-    <t>bei Laune; halten; hält</t>
+    <t>bei; Laune; halten; hält; Luna</t>
   </si>
   <si>
     <t>ph00077</t>
@@ -2770,7 +2770,7 @@
     <t>Irgendwann muss auch jeder den Löffel abgeben.</t>
   </si>
   <si>
-    <t xml:space="preserve">den Löffel; abgeben; abgegeben; hat; </t>
+    <t>den Löffel; abgeben; abgegeben; hat; Löffel;</t>
   </si>
   <si>
     <t>ph00079</t>
@@ -2941,7 +2941,7 @@
     <t>Sie ist vernarrt in ihren neuen Hund und redet nur noch von ihm.</t>
   </si>
   <si>
-    <t>einen Narren; an; gefressen; haben; hast; hat; ist vernarrt in;</t>
+    <t>einen Narren; an; gefressen; haben; hast; hat; ist vernarrt in; vernarrt in jmdn. / etw. sein;</t>
   </si>
   <si>
     <t>ph00084</t>
@@ -3040,7 +3040,7 @@
     <t>Nach stundenlangem Stau lagen bei den Fahrern die Nerven blank, viele hupten und schimpften.</t>
   </si>
   <si>
-    <t xml:space="preserve">Nerven; liegen; blank; lagen; die Nerven; </t>
+    <t>Nerven; liegen; blank; lagen; die Nerven; behalten;</t>
   </si>
   <si>
     <t>ph00087</t>
@@ -3142,7 +3142,7 @@
     <t>Beruhig dich ein bisschen! Komm wieder von der Palme herunter.</t>
   </si>
   <si>
-    <t xml:space="preserve">auf die Palme; bringen; bringt; komm; von der Palme; herunter; </t>
+    <t>auf die Palme; bringen; bringt; komm; von der Palme; herunter; von der Palme wieder herunterkommen;</t>
   </si>
   <si>
     <t>ph00090</t>
@@ -3409,7 +3409,7 @@
     <t>Sie blieb viel zu lange in der Beziehung, obwohl alle Anzeichen zeigten, dass sie nicht mehr funktionierte. Sie hat das tote Pferd geritten, anstatt loszulassen und weiterzugehen.</t>
   </si>
   <si>
-    <t>ein totes Pferd; reiten; wird; hat; geritten</t>
+    <t>ein totes Pferd; reiten; wird; hat; geritten; riding a dead horse</t>
   </si>
   <si>
     <t>ph00098</t>
@@ -3670,7 +3670,7 @@
     <t>Anstatt mit uns zu reden, schmort er lieber allein in seinem eigenen Saft.</t>
   </si>
   <si>
-    <t>im; in; eigenen Saft; schmoren; wirst; schmore; schmort</t>
+    <t>im; in; eigenen Saft; schmoren; wirst; schmore; schmort; jmdn. im eigenen Saft schmoren lassen</t>
   </si>
   <si>
     <t>ph00106</t>
@@ -3766,7 +3766,7 @@
     <t>Er war das schwarze Schaf in der Schule, der immer Ärger machte und sich nicht an die Regeln hielt</t>
   </si>
   <si>
-    <t>schwarzes; das schwarze; Schaf; sein; ist; war</t>
+    <t>schwarzes; das schwarze; Schaf; sein; ist; war; Sündenbock sein, Buhmann sein</t>
   </si>
   <si>
     <t>ph00109</t>
@@ -3868,7 +3868,7 @@
     <t>Du hast das ganze Wochenende nur gelesen? Was bist du denn für eine Schlaftablette?</t>
   </si>
   <si>
-    <t xml:space="preserve">eine; Schlaftablette; sein; ist; Schlaftabletten; sind; </t>
+    <t>eine; Schlaftablette; sein; ist; Schlaftabletten; sind; dröge sein;</t>
   </si>
   <si>
     <t>ph00112</t>
@@ -3964,7 +3964,7 @@
     <t>Wieder so eine olle Kamelle, die jeder kennt und niemand mehr hören will!</t>
   </si>
   <si>
-    <t>Scnhee von gestern; olle Kamelle</t>
+    <t>Scnhee von gestern; olle Kamelle; kalter Kaffee</t>
   </si>
   <si>
     <t>ph00115</t>
@@ -4070,6 +4070,9 @@
     <t>Für das neue Projekt hat kein Schwein Interesse gezeigt.</t>
   </si>
   <si>
+    <t>kein; armes; Schwein</t>
+  </si>
+  <si>
     <t>ph00118</t>
   </si>
   <si>
@@ -4100,7 +4103,7 @@
     <t>Wir hatten wirklich Schwein, dass die Prüfung heute ausgefallen ist und erst nächste Woche stattfindet.</t>
   </si>
   <si>
-    <t>Schwein; haben; gehabt; hatten</t>
+    <t>Schwein; haben; gehabt; hatten; Sau; Schützenfeste;</t>
   </si>
   <si>
     <t>ph00119</t>
@@ -4202,7 +4205,7 @@
     <t>Der psychische Druck während der Prüfungsphase geht vielen Studierenden an die Substanz.</t>
   </si>
   <si>
-    <t xml:space="preserve">an die Substanz; gehen; ging; geht; </t>
+    <t xml:space="preserve">an die; Substanz; gehen; ging; geht; </t>
   </si>
   <si>
     <t>ph00122</t>
@@ -4295,7 +4298,7 @@
     <t xml:space="preserve">Unser Nachbar macht jeden Tag um Mitternacht Lärm in der Garage. Der hat eindeutig nicht alle Tassen im Schrank! </t>
   </si>
   <si>
-    <t xml:space="preserve">nicht alle Tassen im Schrank; haben; hat; habt; </t>
+    <t>nicht alle Tassen im Schrank; haben; hat; habt; eine Macke haben; einen Dachschaden haben; eine Schraube locker haben; nicht alle Latten am Zaun haben; nicht ganz dicht sein;</t>
   </si>
   <si>
     <t>ph00125</t>
@@ -4454,7 +4457,7 @@
     <t>Bei dieser Kälte noch Eis essen? Hast du einen Vogel?</t>
   </si>
   <si>
-    <t>einen Vogel; haben, hat; hast; zeigen; zeigte</t>
+    <t>einen Vogel; haben, hat; hast; zeigen; zeigte; jmdm. einen Vogel zeigen</t>
   </si>
   <si>
     <t>ph00130</t>
@@ -4487,7 +4490,7 @@
     <t>Du hast doch einen an der Waffel, so etwas macht man nicht.</t>
   </si>
   <si>
-    <t xml:space="preserve">einen an der Waffel; haben; hast; </t>
+    <t>einen an der; Waffel; haben; hast; waffeln; waffle</t>
   </si>
   <si>
     <t>ph00131</t>
@@ -4547,7 +4550,7 @@
     <t>Manchmal muss man einfach mutig sein und ins kalte Wasser springen – sonst entwickelt man sich nicht weiter.</t>
   </si>
   <si>
-    <t xml:space="preserve">ins kalte Wasser; springen; </t>
+    <t>ins kalte Wasser; springen; jmdn. ins kalte Wasser werfen/schmeißen;</t>
   </si>
   <si>
     <t>ph00133</t>
@@ -4580,7 +4583,7 @@
     <t>Der Lehrer hat beim Abschied fast geweint – er ist eben nah am Wasser gebaut.</t>
   </si>
   <si>
-    <t>nah am Wasser; gebaut; sein; bin; war; ist;</t>
+    <t xml:space="preserve">nah am Wasser; gebaut; sein; bin; war; ist; Heulsuse; </t>
   </si>
   <si>
     <t>ph00134</t>
@@ -4775,7 +4778,7 @@
     <t>So kann ich nicht ins Restaurant gehen – ich sehe aus wie durch den Fleischwolf gedreht.</t>
   </si>
   <si>
-    <t xml:space="preserve">sich; fühlen; wie durch den Wolf; gedreht; fühle; mich; </t>
+    <t>sich; fühlen; wie durch den Wolf; gedreht; fühle; mich; durch den; Fleischwolf</t>
   </si>
   <si>
     <t>ph00140</t>
@@ -4868,7 +4871,7 @@
     <t>Wir müssen uns alle ins Zeug legen, wenn wir die Deadline einhalten wollen.</t>
   </si>
   <si>
-    <t>sich; für; ins Zeug; legen; dich; uns</t>
+    <t>sich; für; ins Zeug; legen; dich; uns; sich für jmdn. ins Zeug legen</t>
   </si>
 </sst>
 </file>
@@ -12920,7 +12923,7 @@
       </c>
       <c r="R117" s="1"/>
       <c r="S117" s="1" t="s">
-        <v>1323</v>
+        <v>1332</v>
       </c>
       <c r="T117" s="2"/>
       <c r="U117" s="2"/>
@@ -12937,22 +12940,22 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>560</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="G118" s="4" t="s">
         <v>26</v>
@@ -12964,28 +12967,28 @@
         <v>29</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="L118" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M118" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="O118" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="P118" s="1"/>
       <c r="Q118" s="1"/>
       <c r="R118" s="1"/>
       <c r="S118" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="T118" s="2"/>
       <c r="U118" s="2"/>
@@ -13002,28 +13005,28 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="G119" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>29</v>
@@ -13032,27 +13035,27 @@
         <v>29</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="L119" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M119" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="O119" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="P119" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
       <c r="S119" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="T119" s="2"/>
       <c r="U119" s="2"/>
@@ -13069,19 +13072,19 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>523</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>263</v>
@@ -13099,27 +13102,27 @@
         <v>29</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="L120" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M120" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="O120" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="P120" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="Q120" s="1"/>
       <c r="R120" s="1"/>
       <c r="S120" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="T120" s="2"/>
       <c r="U120" s="2"/>
@@ -13136,13 +13139,13 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>884</v>
@@ -13151,13 +13154,13 @@
         <v>884</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="I121" s="1" t="s">
         <v>29</v>
@@ -13166,27 +13169,27 @@
         <v>29</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="L121" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M121" s="1" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="O121" s="1" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="P121" s="1" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="Q121" s="1"/>
       <c r="R121" s="1"/>
       <c r="S121" s="1" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="T121" s="2"/>
       <c r="U121" s="2"/>
@@ -13203,19 +13206,19 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>319</v>
@@ -13230,28 +13233,28 @@
         <v>562</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="L122" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M122" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="O122" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="P122" s="1"/>
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
       <c r="S122" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="T122" s="2"/>
       <c r="U122" s="2"/>
@@ -13268,13 +13271,13 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>174</v>
@@ -13289,34 +13292,34 @@
         <v>26</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="J123" s="1" t="s">
         <v>29</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="L123" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M123" s="1" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="O123" s="1" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="P123" s="1"/>
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
       <c r="S123" s="1" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="T123" s="2"/>
       <c r="U123" s="2"/>
@@ -13333,16 +13336,16 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
@@ -13354,7 +13357,7 @@
         <v>26</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>29</v>
@@ -13363,25 +13366,25 @@
         <v>29</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="L124" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M124" s="1" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="O124" s="1" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="P124" s="1"/>
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
       <c r="S124" s="1" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="T124" s="2"/>
       <c r="U124" s="2"/>
@@ -13398,19 +13401,19 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>636</v>
@@ -13428,27 +13431,27 @@
         <v>29</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="L125" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M125" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="O125" s="1" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="Q125" s="1"/>
       <c r="R125" s="1"/>
       <c r="S125" s="1" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="T125" s="2"/>
       <c r="U125" s="2"/>
@@ -13465,22 +13468,22 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>149</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="G126" s="4" t="s">
         <v>26</v>
@@ -13492,28 +13495,28 @@
         <v>29</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="L126" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M126" s="1" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="N126" s="1" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="O126" s="1" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="P126" s="1"/>
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
       <c r="S126" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="T126" s="2"/>
       <c r="U126" s="2"/>
@@ -13530,19 +13533,19 @@
     </row>
     <row r="127">
       <c r="A127" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>623</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>319</v>
@@ -13566,21 +13569,21 @@
         <v>29</v>
       </c>
       <c r="M127" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="N127" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="O127" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="P127" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="Q127" s="1"/>
       <c r="R127" s="1"/>
       <c r="S127" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="T127" s="2"/>
       <c r="U127" s="2"/>
@@ -13597,13 +13600,13 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>623</v>
@@ -13618,7 +13621,7 @@
         <v>26</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="I128" s="1" t="s">
         <v>551</v>
@@ -13627,29 +13630,29 @@
         <v>29</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="L128" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M128" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="O128" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="P128" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="Q128" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="R128" s="1"/>
       <c r="S128" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="T128" s="2"/>
       <c r="U128" s="2"/>
@@ -13666,19 +13669,19 @@
     </row>
     <row r="129">
       <c r="A129" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>613</v>
@@ -13687,36 +13690,36 @@
         <v>26</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="I129" s="1" t="s">
         <v>29</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="L129" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M129" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="N129" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="O129" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="P129" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="Q129" s="1"/>
       <c r="R129" s="1"/>
       <c r="S129" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="T129" s="2"/>
       <c r="U129" s="2"/>
@@ -13733,19 +13736,19 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>29</v>
@@ -13754,34 +13757,34 @@
         <v>26</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="J130" s="1" t="s">
         <v>29</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="L130" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M130" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="N130" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="O130" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="P130" s="1"/>
       <c r="Q130" s="1"/>
       <c r="R130" s="1"/>
       <c r="S130" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="T130" s="2"/>
       <c r="U130" s="2"/>
@@ -13798,22 +13801,22 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>862</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="G131" s="4" t="s">
         <v>26</v>
@@ -13828,25 +13831,25 @@
         <v>29</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="L131" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M131" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="N131" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="O131" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="P131" s="1"/>
       <c r="Q131" s="1"/>
       <c r="R131" s="1"/>
       <c r="S131" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="T131" s="2"/>
       <c r="U131" s="2"/>
@@ -13863,19 +13866,19 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>547</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>365</v>
@@ -13884,7 +13887,7 @@
         <v>26</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>29</v>
@@ -13893,25 +13896,25 @@
         <v>29</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="L132" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M132" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="N132" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="O132" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="P132" s="1"/>
       <c r="Q132" s="1"/>
       <c r="R132" s="1"/>
       <c r="S132" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="T132" s="2"/>
       <c r="U132" s="2"/>
@@ -13928,19 +13931,19 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>263</v>
@@ -13949,7 +13952,7 @@
         <v>26</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="I133" s="1" t="s">
         <v>29</v>
@@ -13958,25 +13961,25 @@
         <v>29</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="L133" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M133" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="N133" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="O133" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="P133" s="1"/>
       <c r="Q133" s="1"/>
       <c r="R133" s="1"/>
       <c r="S133" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="T133" s="2"/>
       <c r="U133" s="2"/>
@@ -13993,13 +13996,13 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>163</v>
@@ -14020,28 +14023,28 @@
         <v>29</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="L134" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M134" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="N134" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="O134" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="P134" s="1"/>
       <c r="Q134" s="1"/>
       <c r="R134" s="1"/>
       <c r="S134" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="T134" s="2"/>
       <c r="U134" s="2"/>
@@ -14058,19 +14061,19 @@
     </row>
     <row r="135">
       <c r="A135" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>399</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>560</v>
@@ -14079,7 +14082,7 @@
         <v>26</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="I135" s="1" t="s">
         <v>29</v>
@@ -14088,25 +14091,25 @@
         <v>29</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="L135" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M135" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="N135" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="O135" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="P135" s="1"/>
       <c r="Q135" s="1"/>
       <c r="R135" s="1"/>
       <c r="S135" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="T135" s="2"/>
       <c r="U135" s="2"/>
@@ -14123,16 +14126,16 @@
     </row>
     <row r="136">
       <c r="A136" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>961</v>
@@ -14153,27 +14156,27 @@
         <v>29</v>
       </c>
       <c r="K136" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="L136" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M136" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="N136" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="O136" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="P136" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="Q136" s="1"/>
       <c r="R136" s="1"/>
       <c r="S136" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="T136" s="2"/>
       <c r="U136" s="2"/>
@@ -14190,28 +14193,28 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>884</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="G137" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="I137" s="1" t="s">
         <v>551</v>
@@ -14220,27 +14223,27 @@
         <v>29</v>
       </c>
       <c r="K137" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="L137" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M137" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="N137" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="O137" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="P137" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="Q137" s="1"/>
       <c r="R137" s="1"/>
       <c r="S137" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="T137" s="2"/>
       <c r="U137" s="2"/>
@@ -14257,28 +14260,28 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="G138" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="I138" s="1" t="s">
         <v>551</v>
@@ -14287,27 +14290,27 @@
         <v>29</v>
       </c>
       <c r="K138" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="L138" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M138" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="N138" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="O138" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="P138" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="Q138" s="1"/>
       <c r="R138" s="1"/>
       <c r="S138" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="T138" s="2"/>
       <c r="U138" s="2"/>
@@ -14324,19 +14327,19 @@
     </row>
     <row r="139">
       <c r="A139" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>884</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>200</v>
@@ -14345,25 +14348,25 @@
         <v>26</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="L139" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M139" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="N139" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="O139" s="1" t="s">
         <v>29</v>
@@ -14372,7 +14375,7 @@
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
       <c r="S139" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="T139" s="2"/>
       <c r="U139" s="2"/>
@@ -14389,13 +14392,13 @@
     </row>
     <row r="140">
       <c r="A140" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>623</v>
@@ -14419,29 +14422,29 @@
         <v>625</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="L140" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M140" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="N140" s="1" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="O140" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="P140" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="Q140" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="R140" s="1"/>
       <c r="S140" s="1" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="T140" s="2"/>
       <c r="U140" s="2"/>
@@ -14458,13 +14461,13 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>904</v>
@@ -14473,7 +14476,7 @@
         <v>905</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="G141" s="4" t="s">
         <v>26</v>
@@ -14485,28 +14488,28 @@
         <v>29</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="L141" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M141" s="1" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="N141" s="1" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="O141" s="1" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="P141" s="1"/>
       <c r="Q141" s="1"/>
       <c r="R141" s="1"/>
       <c r="S141" s="1" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="T141" s="2"/>
       <c r="U141" s="2"/>
@@ -14523,19 +14526,19 @@
     </row>
     <row r="142">
       <c r="A142" s="1" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>355</v>
@@ -14544,7 +14547,7 @@
         <v>26</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="I142" s="1" t="s">
         <v>551</v>
@@ -14553,25 +14556,25 @@
         <v>29</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="L142" s="1" t="s">
         <v>29</v>
       </c>
       <c r="M142" s="1" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="O142" s="1" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="P142" s="1"/>
       <c r="Q142" s="1"/>
       <c r="R142" s="1"/>
       <c r="S142" s="1" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="T142" s="2"/>
       <c r="U142" s="2"/>

</xml_diff>

<commit_message>
Alle Beispiele; Kursive und Graue Markierung
</commit_message>
<xml_diff>
--- a/tabelle_1_main.xlsx
+++ b/tabelle_1_main.xlsx
@@ -174,7 +174,7 @@
     <t>auf; abfahren; abgefahren; fährt; ab; etw. ist abgefahren</t>
   </si>
   <si>
-    <t xml:space="preserve">15.02.2026: alle Beispiele hinzugefügt und kursiv markiert </t>
+    <t>15.02.2026_2130: alle Beispiele hinzugefügt, kursiv und grau markiert</t>
   </si>
   <si>
     <t>ph00002</t>
@@ -198,7 +198,7 @@
     <t>Ихэвчлэн эгэх төлөөний үгтэй (Refl.) хэрэглэнэ</t>
   </si>
   <si>
-    <t>онигоонд орох, хөгөө чирэх, шараа болох</t>
+    <t>онигоонд орох; хөгөө чирэх; шараа болох</t>
   </si>
   <si>
     <t>Mach dich nicht zum Affen und benimm dich einfach normal.</t>
@@ -234,7 +234,7 @@
     <t>Spaß machen, jmdn. verarschen, jmdn. veräppeln мөн адил утгатай.</t>
   </si>
   <si>
-    <t>хэн нэгнийг явуулах, цаашлуулах, тоглоом тохуу хийх</t>
+    <t>хэн нэгнийг явуулах; цаашлуулах; тоглоом тохуу хийх</t>
   </si>
   <si>
     <t>So viel Geld für Kleidung ausgegeben!? Willst du mich auf den Arm nehmen?</t>
@@ -279,7 +279,7 @@
     <t>Дундад зуунд өргөн ханцуйтай хувцас моод байсан бөгөөд илбэчид үзүүлбэртээ ханцуйнаасаа гэнэт төрөл бүрийн зүйл гаргаж ирдэг байснаас  үүсэлтэй.</t>
   </si>
   <si>
-    <t>нүд ирмэх зуур, алга хөрвүүлэхийн хооронд, etw. aus der Hand schütteln / zaubern, etw. aus dem Handgelenk schütteln / zaubern</t>
+    <t>нүд ирмэх зуур; алга хөрвүүлэхийн хооронд; etw. aus der Hand schütteln / zaubern; etw. aus dem Handgelenk schütteln / zaubern</t>
   </si>
   <si>
     <t>Bei der Besprechung hat er plötzlich eine brillante Idee aus dem Ärmel geschüttelt.</t>
@@ -316,7 +316,7 @@
     <t>Хүн хэхрэхэд таагүй, гашуун мэдрэмж буюу цээж хорсож байгаатай адилтгасан зүйрлэл.</t>
   </si>
   <si>
-    <t>дургүй хүрэх, зэвүүцэх, übel aufstoßen</t>
+    <t>дургүй хүрэх; зэвүүцэх; übel aufstoßen</t>
   </si>
   <si>
     <t>Es stößt mir sauer auf, dass er nie seine Versprechen hält.</t>
@@ -391,7 +391,7 @@
     <t>Хэн нэгэнд таалагдах зорилготой учраас өгөх оршихын тийн ялгалд (Dat.) байгаа эзэн биеийг заавал дурьдна.</t>
   </si>
   <si>
-    <t>хэн нэгэнд хандрах, харц чулуудах</t>
+    <t>хэн нэгэнд хандрах; харц чулуудах</t>
   </si>
   <si>
     <t>Hör auf, Lisa schöne Augen zu machen, du hast doch eine Freundin!</t>
@@ -529,7 +529,7 @@
     <t>Schiss haben гэх хэлцтэй утгын хувьд адил боловч хэрэглээний хувьд ялгаатай. Schiss haben гэдэг нь илүү хүчтэй айдас илэрхийлэх бол Bammel haben нь утгын хувьд хүч султайгаас гадна ихэвчилэн нөхцөл байдлаас үүдсэн тодорхой бус айдсыг илэрхийлнэ.</t>
   </si>
   <si>
-    <t>зүрх үхэх, зүрхлэхгүй байх</t>
+    <t>зүрх үхэх; зүрхлэхгүй байх</t>
   </si>
   <si>
     <t>Ich habe Bammel, in den Keller zu gehen.</t>
@@ -568,7 +568,7 @@
     <t>Barrikade гэдэг нь франц гаралтай үг бөгөөд 18-р зууны Францын хувьсгалын үеэр ард түмэн хаант засаглалын эсрэг босохдоо хаалт, хамгаалалт барьж эсэргүүцэж байснаас үүдэлтэй.</t>
   </si>
   <si>
-    <t>бослого гаргах, эсэргүүцэн тэмцэх</t>
+    <t>бослого гаргах; эсэргүүцэн тэмцэх</t>
   </si>
   <si>
     <t>Die Bürger gingen auf die Barrikaden, als die Regierung die Steuern erhöhte.</t>
@@ -604,7 +604,7 @@
     <t>Дундад зуунд театрын жүжигчид тоглолт дээрээ ёс бус, садар самуун утгатай үг болон хориотой зүйлийн талаар ярихдаа болгоомжилон, танигдахгүйн тулд амныхаа урд цаас эсвэл даавуу барьдаг байжээ.</t>
   </si>
   <si>
-    <t>улаан хэлтнийг урдуураа өнгөрөөхгүй, нүүрэн дээр нь хэлэх</t>
+    <t>улаан хэлтнийг урдуураа өнгөрөөхгүй; нүүрэн дээр нь хэлэх</t>
   </si>
   <si>
     <t>Sie nimmt kein Blatt vor den Mund, sie sagt immer, was sie denkt.</t>
@@ -679,7 +679,7 @@
     <t>blau vor den Augen werden хэлцтэй холбоотой. Энэ нь толгой эргэж, дайвалзах, нүд бүрэлзэх гэсэн утгатай.</t>
   </si>
   <si>
-    <t xml:space="preserve">хөлчүү байх, хөлчүүрхэх, мал болтлоо согтох, тасрах, нохой дөрөв харагдах </t>
+    <t xml:space="preserve">хөлчүү байх; хөлчүүрхэх; мал болтлоо согтох; тасрах; нохой дөрөв харагдах </t>
   </si>
   <si>
     <t>Du warst gestern Abend ganz schön blau. Kannst du dich überhaupt noch an etwas erinnern?</t>
@@ -754,7 +754,7 @@
     <t>den Boden unter den Füßen verlieren гэх хэлцтэй утгын хувьд адил.  Монгол хэлний хөл алдах гэдэг хэлцтэй андуурч болохгүй.</t>
   </si>
   <si>
-    <t>хөл доорх газар цөмрөх, сэтгэлээр унах, элэг эмтрэх</t>
+    <t>хөл доорх газар цөмрөх; сэтгэлээр унах; элэг эмтрэх</t>
   </si>
   <si>
     <t>Nachdem er seine Frau verloren hat, war er am Boden zerstört.</t>
@@ -796,7 +796,7 @@
     <t>20-р зууны дунд үед англи хэлнээс орж ирсэн to be in the same boat хэллэгийн утгачилсан орчуулга бөгөөд далайчид нэг завинд нэг л хувь тавилан хуваалцдаг амьдралаас үүдэлтэй.</t>
   </si>
   <si>
-    <t>im selben Boot sitzen, in einem Boot sitzen, зовлон нэгтэй байх</t>
+    <t>im selben Boot sitzen; in einem Boot sitzen; зовлон нэгтэй байх</t>
   </si>
   <si>
     <t>Die Schüler im letzten Jahrgang sitzen im gleichen Boot – alle müssen die Abschlussprüfung bestehen.</t>
@@ -832,7 +832,7 @@
     <t>wie die Katze um den heißen Brei schleichen гэсэн хуучны хэлцээс гаралтай. Муур халуун зутан идэж чадахгүй тойрон гэтэх үйлтэй зүйрлэсэн хэлц үг.</t>
   </si>
   <si>
-    <t>зайлсхийх, тойруулж ярих, дүлэгнэх</t>
+    <t>зайлсхийх; тойруулж ярих; дүлэгнэх</t>
   </si>
   <si>
     <t>Hör auf, immer um den heißen Brei zu reden, sag mir endlich, was du wirklich denkst!</t>
@@ -862,7 +862,7 @@
     <t>Emotion</t>
   </si>
   <si>
-    <t>уураа гаргах, бухимдлаа тайлах</t>
+    <t>уураа гаргах; бухимдлаа тайлах</t>
   </si>
   <si>
     <t>Nach dem Streit ging sie zum Fitness-Studio, um endlich Dampf abzulassen.</t>
@@ -871,7 +871,7 @@
     <t>Wenn du Dampf ablassen musst, ruf mich an – ich höre dir zu.</t>
   </si>
   <si>
-    <t xml:space="preserve">Damof; ablassen; abzulassen; </t>
+    <t xml:space="preserve">Dampf; ablassen; abzulassen; </t>
   </si>
   <si>
     <t>ph00021</t>
@@ -898,7 +898,7 @@
     <t>Эртний Ромчууд гладиаторуудын амь насыг шийдэх өршөөлийн дохиог эрхий хуруугаар илэрхийлдэг байжээ. Гладиатор тулаанд ялагдвал долоовор хуруугаа өргөн үзэгчдээс өршөөл хүсдэг байсан бөгөөд тэд гладиаторын үхлийг хүсвэл гараа сунган эрхий хуруугаа гозойлгон харин түүний амь насыг өршөөх дохио нь эрхий хуруугаа нууж гараа зангидах байв.</t>
   </si>
   <si>
-    <t>амжилт!, toi toi toi, jmdm. ganz fest die Daumen gedrückt, jmdm. alle Daumen drücken</t>
+    <t>амжилт!; toi toi toi; jmdm. ganz fest die Daumen gedrückt; jmdm. alle Daumen drücken</t>
   </si>
   <si>
     <t>Ich habe dir ganz fest die Daumen gedrückt, dass du das Vorstellungsgespräch bestehst.</t>
@@ -913,7 +913,7 @@
     <t>Ich drücke dir die Daumen für dein neues Projekt. Viel Erfolg!</t>
   </si>
   <si>
-    <t xml:space="preserve">die Daumen; drücken; habe; gedrückt; drücke; </t>
+    <t xml:space="preserve">die Daumen; alle Daumen; drücken; habe; gedrückt; drücke; </t>
   </si>
   <si>
     <t>ph00022</t>
@@ -925,7 +925,7 @@
     <t>дүрсхийн уурлах, огцом уурлах, түргэн зан гаргах</t>
   </si>
   <si>
-    <t>sehr schnell an die Decke gehen, тэсрэх, зүрхний хийтэй, боож үхэхээ шахах</t>
+    <t>sehr schnell an die Decke gehen; тэсрэх, зүрхний хийтэй; боож үхэхээ шахах</t>
   </si>
   <si>
     <t>Wenn du ihn provozierst, geht er an die Decke.</t>
@@ -1033,7 +1033,7 @@
     <t>Хэн нэгнийг эсвэл ямар нэгэн зүйлийг ямар ч болзолгүйгээр эрхэмлэн дээдэлж, өөрийн амьдралд чухал байр суурь эзэлж байгааг илэрхийлдэг.</t>
   </si>
   <si>
-    <t>амь, амьдрал байх</t>
+    <t>амь; амьдрал байх</t>
   </si>
   <si>
     <t>Meine Tochter ist mein Ein und Alles.</t>
@@ -1174,7 +1174,7 @@
     <t>Leichtsinn</t>
   </si>
   <si>
-    <t>галаар тоглох, үхлээ эрсэн оготно, муурын сахлаар оролдоно</t>
+    <t>галаар тоглох; үхлээ эрсэн оготно; муурын сахлаар оролдоно</t>
   </si>
   <si>
     <t>Wer so viele Kredite hat, spielt mit dem Feuer und riskiert finanzielle Probleme.</t>
@@ -1210,7 +1210,7 @@
     <t>Найз нөхөд, дотны хүмүүс дундаа хэрэглэхэд илүү тохиромжтой.</t>
   </si>
   <si>
-    <t>кадр тасрах, тас үсрэх, тасрах</t>
+    <t>кадр тасрах; тас үсрэх; тасрах</t>
   </si>
   <si>
     <t>Ich war gestern total betrunken und kann mich nur bruchstückhaft erinnern, was ich gemacht habe. Ich habe total den Filmriss!</t>
@@ -1222,7 +1222,7 @@
     <t>Nach dem Unfall hatte ich einen Filmriss, ich kann mich nicht erinnern, was passiert ist.</t>
   </si>
   <si>
-    <t>einen Filmriss; den Filmriss; haben; habe; hatte</t>
+    <t>einen Filmriss; den Filmriss; haben; habe total; hatte</t>
   </si>
   <si>
     <t>ph00031</t>
@@ -1246,7 +1246,7 @@
     <t>Анчид байгаа оноогүй үедээ уурлан буугаа чулуудах нь нэгэнт зорилгодоо хүрч чадахгүй гэдгээ хүлээн зөвшөөрч, шантрахыг илтгэдэг байжээ.</t>
   </si>
   <si>
-    <t>бууж өгөх, шантрах</t>
+    <t>бууж өгөх; шантрах</t>
   </si>
   <si>
     <t>Er hat die Flinte ins Korn geworfen und wollte sein Studium abbrechen, weil er die Prüfung nicht bestanden hat.</t>
@@ -1273,7 +1273,7 @@
     <t>Маш их баярлаж байгаа байдал илт харагдах. Энэхүү хэллэг нь ихэвчлэн спорт, тэмцээн, шалгалтад амжилт гарсан эсвэл бэлэг авах, гэнэтийн сайхан зүйл тохиолдсон үед ашиглагддаг.</t>
   </si>
   <si>
-    <t>хөл газар хүрэхгүй баярлах, магнай тэнийх</t>
+    <t>хөл газар хүрэхгүй баярлах; магнай тэнийх</t>
   </si>
   <si>
     <t>Als sie die Konzerttickets bekam, sprang er vor Freude an die Decke.</t>
@@ -1306,7 +1306,7 @@
     <t>Чухал шийдвэр гаргахын өмнө эргэлзэж, эмээж буйгаа энэ хэлцээр илэрхийлж болно.</t>
   </si>
   <si>
-    <t>халшрах, jmdm. nicht mehr geheuer sein, ein mulmiges Gefühl bekommen</t>
+    <t>халшрах; jmdm. nicht mehr geheuer sein; ein mulmiges Gefühl bekommen</t>
   </si>
   <si>
     <t>Ich hoffe, dass er nicht im letzten Moment kalte Füße bekommt und seinen Vortrag absagt.</t>
@@ -1327,7 +1327,7 @@
     <t>Bei dem Gespräch mit meinem Chef hatte ich ein mulmiges Gefühl.</t>
   </si>
   <si>
-    <t xml:space="preserve">kalte Füße; bekommen; kriegen; bekommt; wird; bin; nicht geheuer; ein mulmiges Gefühl, hatte </t>
+    <t xml:space="preserve">kalte Füße; bekommen; kriegen; bekommt; wird; bin; nicht geheuer; ein mulmiges Gefühl; hatte </t>
   </si>
   <si>
     <t>ph00034</t>
@@ -1345,7 +1345,7 @@
     <t>Монгол хэлэнд цөс хөөрөх нь мөн аархах, онгирох гэсэн утга илэрхийлдэг тул андуурч болохгүй.</t>
   </si>
   <si>
-    <t>уурласнаас болж цөс нь хөөрөх, jmdm. läuft die Galle über</t>
+    <t>уурласнаас болж цөс нь хөөрөх; jmdm. läuft die Galle über</t>
   </si>
   <si>
     <t>Als er hörte, wie sein Kollege die Schuld auf ihn schob, kam ihm die Galle hoch.</t>
@@ -1417,7 +1417,7 @@
     <t>Дундад зууны үед нас барж буй хүний аманд өвс эсвэл шороо хийдэг нэгэн төрлийн заншил байснаас энэхүү хэллэг үүссэн гэж үздэг.</t>
   </si>
   <si>
-    <t>чад хийх, чадрах</t>
+    <t>чад хийх; чадрах</t>
   </si>
   <si>
     <t>Nach dem Unfall wusste jeder, dass er ins Gras gebissen hat.</t>
@@ -1447,7 +1447,7 @@
     <t>1990-д оноос хэрэглэгдэж эхэлсэн бөгөөд ногоон өнгө нь тоног төхөөрөмжийн хэвийн үйл ажиллагааг илэрхийлдэг.</t>
   </si>
   <si>
-    <t>alles in Ordnung, alles okay, гайгүй, тайвандаа</t>
+    <t xml:space="preserve">гайгүй; тайвандаа; alles in Ordnung; alles okay; </t>
   </si>
   <si>
     <t>Bei mir ist alles im grünen Bereich und ich bin jetzt wirklich glücklich.</t>
@@ -1486,7 +1486,7 @@
     <t>Энэ хэлц үг нь 19-р зууны театрын хэллэгээс үүссэн гэдэг. Хоолойгоо хэтэрхий хүчилж, шахаж дуулах буюу ярихыг knödeln гэдэг бөгөөд дуурийн дуучныг егөөдөн Knödeltenor гэж нэрлэдэг байна.</t>
   </si>
   <si>
-    <t>хоолой зангирах, гол горойх</t>
+    <t>хоолой зангирах; гол горойх</t>
   </si>
   <si>
     <t>Als sie ihre Dankesrede hielt, hatte sie einen Kloß im Hals und konnte kaum sprechen.</t>
@@ -1549,7 +1549,7 @@
     <t>Хүний арьс хүний биеийг бүрхдэг хамгийн том эрхтэн юм. Nicht aus seiner Haut können гэдгээр хүн зан чанар, үзэл бодолоо өөрчилж чадахгүй буюу “өөрийн арьснаас гарч чадахгүй” гэсэн утгатай бол aus der Haut fahren гэдэг нь “арьснаасаа гартлаа” асар их уурлахыг хэлнэ.</t>
   </si>
   <si>
-    <t>галзууртлаа уурлах, нүд нь улаанаар эргэлдэх, цөс буцлах</t>
+    <t>галзууртлаа уурлах; нүд нь улаанаар эргэлдэх; цөс буцлах</t>
   </si>
   <si>
     <t>Früher bin ich häufig aus der Haut gefahren, wenn ich wütend wurde, und habe anschließend bereut, was ich gesagt habe.</t>
@@ -1582,7 +1582,7 @@
     <t>Библид “Ертөнцийн эзэнд итгэж түүнд зүрх сэтгэлээ уудла, тэр үргэлж бидний талд” гэжээ. Сэтгэл доторх нуугдсан мэдрэмжүүдийг агуулдаг “сав”-ыг зүрхээр төлөөлөн илэрхийлсэн байна.</t>
   </si>
   <si>
-    <t>сэтгэлээ уудлах, сэтгэлээ нээх</t>
+    <t>сэтгэлээ уудлах; сэтгэлээ нээх</t>
   </si>
   <si>
     <t>Obwohl sie normalerweise sehr verschlossen ist, hat sie ihm gestern ihr Herz ausgeschüttet und von ihren Ängsten erzählt.</t>
@@ -1615,7 +1615,7 @@
     <t>Энэ хэлц нь 17-р зуунд бичгээр тэмдэглэгдсэн ба зүрх нь сэтгэл хөдлөлийн төв гэсэн утга агуулдаг. Хэн нэгэн эсвэл ямар нэг зүйл “зүрхний нэг хэсэг болсон” гэсэн ойлголтоос үүдэлтэй.</t>
   </si>
   <si>
-    <t>бие биедээ дасах, зүрхний угаас хайрлах</t>
+    <t>бие биедээ дасах; зүрхний угаас хайрлах</t>
   </si>
   <si>
     <t>Mein Hund ist mir über die Jahre sehr ans Herz gewachsen.</t>
@@ -1651,7 +1651,7 @@
     <t>Өгүүлэгдэхүүн гишүүн нь үргэлж өгөх оршихын тийн ялгалд (Dat.) байна.</t>
   </si>
   <si>
-    <t>өр зүрх урагдах, зүрх зүүгээр шивэх шиг болох, зүрх зүсэх, элэг эмтрэх</t>
+    <t>өр зүрх урагдах; зүрх зүүгээр шивэх шиг болох; зүрх зүсэх; элэг эмтрэх</t>
   </si>
   <si>
     <t>Mir blutet das Herz, wenn ich jemanden sehe, der auf der Straße lebt.</t>
@@ -1687,7 +1687,7 @@
     <t>Өгүүлэгдэхүүн гишүүн нь үр- гэлж өгөх оршихын тийн ялгалд (Dat.) байна.</t>
   </si>
   <si>
-    <t>нуруун дээрээс ачаа авч хаях, сэтгэл хөнгөрөх</t>
+    <t>нуруун дээрээс ачаа авч хаях; сэтгэл хөнгөрөх</t>
   </si>
   <si>
     <t>Der Arzt hat gesagt, die Operation sei gut verlaufen. Da ist mir ein Stein vom Herzen gefallen.</t>
@@ -1726,7 +1726,7 @@
     <t>Эгэх төлөөний үгтэй (Refl.) хэрэглэнэ.</t>
   </si>
   <si>
-    <t>зүрх гаргах, зүрх орох</t>
+    <t>зүрх гаргах; зүрх орох</t>
   </si>
   <si>
     <t>Er nimmt sich ein Herz und gesteht ihr seine Liebe.</t>
@@ -1759,7 +1759,7 @@
     <t>Өгөх оршихын тийн ялгалд (Dat.) хэрэглэнэ.</t>
   </si>
   <si>
-    <t>нар гарах, магнай тэнийх</t>
+    <t>нар гарах; магнай тэнийх</t>
   </si>
   <si>
     <t>Als sie ihre Familie nach langer Zeit wiedersah, ging ihr das Herz auf.</t>
@@ -1816,7 +1816,7 @@
     <t>Schreck</t>
   </si>
   <si>
-    <t>зүрх пал хийх, зүрх авах, jmdm. fällt das Herz in die Hose, jmdm. sinkt das Herz in die Hose</t>
+    <t>зүрх пал хийх; зүрх авах; jmdm. fällt das Herz in die Hose; jmdm. sinkt das Herz in die Hose</t>
   </si>
   <si>
     <t>Jedes Mal, wenn der Lehrer nach den Hausaufgaben fragt, rutscht mir das Herz in die Hose.</t>
@@ -1852,7 +1852,7 @@
     <t>уран зохиолын хэл</t>
   </si>
   <si>
-    <t>хэн нэгэнд зүрх сэтгэлээ өгөх, хөлөө хугалчих шахах</t>
+    <t>хэн нэгэнд зүрх сэтгэлээ өгөх; хөлөө хугалчих шахах</t>
   </si>
   <si>
     <t>Sie merkt nicht einmal, dass er ihr längst sein Herz zu Füßen gelegt hat.</t>
@@ -1948,7 +1948,7 @@
     <t>Эртний одон орны ухаанд долоон гараг байдаг гэж үздэг байв. Долоо дахь тэнгэр нь хамгийн дээд, ариун бөгөөд ингэснээр хамгийн дээд аз жаргалд хүрэхийг илтгэдэг  байжээ.</t>
   </si>
   <si>
-    <t>жаргалдаа умбах, баярын нар гарах, нисэх шахах</t>
+    <t>жаргалдаа умбах; баярын нар гарах; нисэх шахах</t>
   </si>
   <si>
     <t>Seitdem er verliebt ist, ist er im siebten Himmel.</t>
@@ -2020,7 +2020,7 @@
     <t>Эрт үед хүмүүс баавгайн өмсгөл өмсөж зөгийн үүрнээс бал авахдаа зөгийг хуурахын тулд өмсгөлийн аманд бал түрхдэг байжээ.</t>
   </si>
   <si>
-    <t>цаасан малгай өмсгөх, тал засах, jmdm. Honig ums Maul schmieren</t>
+    <t>цаасан малгай өмсгөх; тал засах; jmdm. Honig ums Maul schmieren</t>
   </si>
   <si>
     <t>Er hat der Chefin wieder Honig um den Mund geschmiert, nur damit sie ihm das neue Projekt gibt.</t>
@@ -2089,7 +2089,7 @@
     <t>auf den Hund kommen хэлц нь амьдрал, эрүүл мэнд, ажил хэрэг эсвэл эдийн засгийн байдал муудах, доройтох, сүйрэх гэсэн утгатай.</t>
   </si>
   <si>
-    <t>нохойн замаар оруулах/орох, буруу замаар будаа тээлгэх / тээх</t>
+    <t>нохойн замаар оруулах / орох; буруу замаар будаа тээлгэх / тээх</t>
   </si>
   <si>
     <t>Wenn das so weitergeht, bringt dich dein Lebensstil noch auf den Hund.</t>
@@ -2191,7 +2191,7 @@
     <t>Энэхүү хэлцийг зөвхөн сэтгэл санааны хувьд гутралд орсон үед бус, нийгэм, эдийн засаг, байгууллагын санхүүгийн байдал гэх мэт нөхцөл байдалд хэрэглэж болно.</t>
   </si>
   <si>
-    <t>сүйрлийн ирмэгт очих, адагтаа тулах, тартагтаа тулах, модоо барих</t>
+    <t>сүйрлийн ирмэгт очих; адагтаа тулах; тартагтаа тулах; модоо барих</t>
   </si>
   <si>
     <t>Die Ehe von den beiden ist vor die Hunde gegangen, sie haben sich scheiden lassen.</t>
@@ -2230,7 +2230,7 @@
     <t>“kalt” буюу “хүйтэн” гэдэг нь хүн нас барсны дараа бие нь хөрдөгтэй холбоотой үүссэн үг.</t>
   </si>
   <si>
-    <t>амийг нь хорлох, егүүтгэх, таслах, цааш нь харуулах</t>
+    <t>амийг нь хорлох; егүүтгэх, таслах; цааш нь харуулах</t>
   </si>
   <si>
     <t>Wenn er das herausfindet, dass du sein Auto kaputt gemacht hast, macht er dich kalt.</t>
@@ -2263,7 +2263,7 @@
     <t>Дундад зуунд нийтийн халуун усны газарт Bader хэмээх мэргэжилтэй хүн ажилладаг байжээ. Тэрээр үс, сахал засах, бумба тавих, шарх боох зэрэг олон төрлийн үүрэг гүйцэтгэдэг байв. Ингэхдээ бүх хүний үсийг нэг самаар нэгэн жигд тайрдаг байснаас үүссэн энэ хэлц үгийг одоог хүртэл хэрэглэдэг</t>
   </si>
   <si>
-    <t>бүгдийг нэг шугамаар хэмжих, нэг хэвэнд цутгасан мэт үзэх</t>
+    <t>бүгдийг нэг шугамаар хэмжих; нэг хэвэнд цутгасан мэт үзэх</t>
   </si>
   <si>
     <t>Nicht jeder Jugendliche ist respektlos – man sollte sie nicht über einen Kamm scheren.</t>
@@ -2326,7 +2326,7 @@
     <t>19–р зууны Лейпцигийн оюутнуудын дундах ярианы хэлээс үүсэлтэй. Тэд Katarrh гэдэг үгийг саксон аялгаар Kater гэж дууддаг байжээ. Katarrh нь амьсгалын замын үрэвсэл бөгөөд энэ нь ханиалгах, бие сульдах, толгой өвдөх зэрэг шартахтай адил шинж тэмдгээр илэрдэг.</t>
   </si>
   <si>
-    <t>шартах, зуун за- раа зулзагатайгаа байх</t>
+    <t>шартах; зуун зараа зулзагатайгаа байх</t>
   </si>
   <si>
     <t>Nach der Party hatte er einen schlimmen Kater und lag den ganzen Tag im Bett.</t>
@@ -2338,7 +2338,7 @@
     <t>Heute bin ich total verkatert , denn gestern habe ich meinen Geburtstag gefeiert.</t>
   </si>
   <si>
-    <t>einen Kater; haben; hatte; Katers; bin; verkatert; sein</t>
+    <t>einen; Kater; haben; hatte; Katers; bin; verkatert; sein</t>
   </si>
   <si>
     <t>ph00065</t>
@@ -2449,7 +2449,7 @@
     <t>Klappe нь савны таг гэсэн үг бөгөөд хар ярианд амыг хаах буюу дуугүй болгох гэсэн шилжсэн утгаар хэрэглэдэг. Ихэвчилэн хүнд хандаж хэлэхийн зэрэгцээ 1–р  бие дээр За за яршиг, дугай л байя гэсэн санааг илэрхийлнэ.</t>
   </si>
   <si>
-    <t>олон долоон юм ярихгүй байх, битгий донгос! den Mund halten</t>
+    <t>олон долоон юм ярихгүй байх; битгий донгос!; den Mund halten</t>
   </si>
   <si>
     <t>Wenn du keine Ahnung hast, solltest du einfach mal die Klappe halten.</t>
@@ -2482,7 +2482,7 @@
     <t>klipp und klar нь толгой холбон бүтсэн хэллэг тул байрыг нь сольж болохгүй. Ийм аргаар бүтсэн өөр нэг хэлц нь fix und fertig буюу ядрах, туйлдахыг илэрхийлнэ.</t>
   </si>
   <si>
-    <t>ил тод хэлэх, шу- луухан хэлэх, etw. klipp und klar sagen / machen / erklären / fordern / ablehnen</t>
+    <t>ил тод хэлэх; шулуухан хэлэх; etw. klipp und klar sagen / machen / erklären / fordern / ablehnen</t>
   </si>
   <si>
     <t>Ich habe ihm klipp und klar gesagt, dass unsere Ehe keine Zukunft hat.</t>
@@ -2506,10 +2506,10 @@
     <t>маш их айх, сандрах, сул дорой болох</t>
   </si>
   <si>
-    <t>Энэхүү хэлцийг олон нөхцөл байдалд хэрэглэж болно. Айж эмээх, сэт- гэл догдлох, сэтгэл хөдлөх, цочирдох гэх мэт.</t>
-  </si>
-  <si>
-    <t>өвдөг чичрэх, бүлх залгисан юм шиг болох, weiche Knie kriegen, jmdm. werden die Knie weich</t>
+    <t>Энэхүү хэлцийг олон нөхцөл байдалд хэрэглэж болно. Айж эмээх, сэтгэл догдлох, сэтгэл хөдлөх, цочирдох гэх мэт.</t>
+  </si>
+  <si>
+    <t>өвдөг чичрэх; бүлх залгисан юм шиг болох; weiche Knie kriegen; jmdm. werden die Knie weich</t>
   </si>
   <si>
     <t>Kurz vor der Präsentation bekomme ich immer weiche Knie.</t>
@@ -2542,10 +2542,10 @@
     <t>Vermeidung</t>
   </si>
   <si>
-    <t>Энэ хэлц нь тэмээн хяруултай холбоотой домог, төсөөллөөс үүдэлтэй. Хүмүүс урьд нь тэмээн хяруул аюул тулгарахад айсандаа толгойгоо элсэнд шургуулаад нуугддаг гэж итгэдэг байсан. Энэ нь “аюулыг харахгүй бол байхгүй юм шиг” санагдана гэсэн санаа юм. Иймээс асуудлыг шийдэхийн оронд нуугдаж, мэ- дээгүй юм шиг аашлах хүний үйлдлийг дүйцүүлэн энэ хэлц үүссэн ажээ.</t>
-  </si>
-  <si>
-    <t>нүдэн балай, чихэн дүлий загнах</t>
+    <t>Энэ хэлц нь тэмээн хяруултай холбоотой домог, төсөөллөөс үүдэлтэй. Хүмүүс урьд нь тэмээн хяруул аюул тулгарахад айсандаа толгойгоо элсэнд шургуулаад нуугддаг гэж итгэдэг байсан. Энэ нь “аюулыг харахгүй бол байхгүй юм шиг” санагдана гэсэн санаа юм. Иймээс асуудлыг шийдэхийн оронд нуугдаж, мэдээгүй юм шиг аашлах хүний үйлдлийг дүйцүүлэн энэ хэлц үүссэн ажээ.</t>
+  </si>
+  <si>
+    <t>нүдэн балай; чихэн дүлий загнах</t>
   </si>
   <si>
     <t>Die Firma darf jetzt nicht den Kopf in den Sand stecken – es ist Zeit, die Strategie zu ändern.</t>
@@ -2572,7 +2572,7 @@
     <t>удаан хугацаагаар давчуу орон зайд тусгаарлагдсанаас болж тайван биш байдалд орох, ганцаардах, уйдах, тарчилах, стрессдэх</t>
   </si>
   <si>
-    <t>байж ядах, байж суух газраа олж ядах, jmdm. fällt die Bude auf den Kopf</t>
+    <t>байж ядах; байж суух газраа олж ядах; jmdm. fällt die Bude auf den Kopf</t>
   </si>
   <si>
     <t>Ich bin seit drei Wochen krank im Bett – mir fällt schon die Decke auf den Kopf!</t>
@@ -2584,7 +2584,7 @@
     <t>Dir fällt doch die Decke auf den Kopf, wenn du immer nur zu Hause bist. Geh' doch mal raus!</t>
   </si>
   <si>
-    <t xml:space="preserve">fällt; die Decke auf den Kopf; fiel: </t>
+    <t>fällt; die Decke auf den Kopf; fiel;</t>
   </si>
   <si>
     <t>ph00073</t>
@@ -2662,7 +2662,7 @@
     <t>Stillstand</t>
   </si>
   <si>
-    <t>дороо эргэлдэх, гараас юм гарахгүй байх</t>
+    <t>дороо эргэлдэх; гараас юм гарахгүй байх</t>
   </si>
   <si>
     <t>Wir diskutieren schon seit Stunden über dasselbe Thema und drehen uns nur im Kreis.</t>
@@ -2698,7 +2698,7 @@
     <t>Laune буюу сэтгэл санаа гэх үгийн үндэс латин хэлний Luna буюу сар хэмээх үгээс үүсэлтэй бөгөөд дундад зууны одон орон судлалд сар солигдох нь хүний сэтгэл санаанд хүчтэй нөлөө үзүүлдэг гэж үздэг байжээ.</t>
   </si>
   <si>
-    <t>сэтгэл засах, сэтгэл санааг нь өргөх, сайхан зан хөдөлгөх</t>
+    <t>сэтгэл засах; сэтгэл санааг нь өргөх; сайхан зан хөдөлгөх</t>
   </si>
   <si>
     <t>Er versucht, seinen Chef bei Laune zu halten, indem er besonders fleißig arbeitet.</t>
@@ -2731,7 +2731,7 @@
     <t>Энэхүү хэлц нь үлээвэр хөгжмийн зэмсгээс гаралтай бөгөөд үлээвэр хөгжмийн сүүлийн нүх дээр хамгийн өндөр нот тоглоод түүнээс дээш нот байхгүй учир бүх хүч, боломжоо шавхаж байгаатай зүйрлэжээ.</t>
   </si>
   <si>
-    <t>өрөөлтэй морь гүйцэхээ байх, бүх хүчээ шавхах</t>
+    <t>өрөөлтэй морь гүйцэхээ байх; бүх хүчээ шавхах</t>
   </si>
   <si>
     <t>Nach der Arbeit pfeife ich aus dem letzten Loch. Ich kann einfach nicht mehr.</t>
@@ -2758,7 +2758,7 @@
     <t>Дундад зуунд хүн бүр өөрийн халбагатай байсан бөгөөд хооллох нь амьд яваагийн гол бэлгэ тэмдэг байжээ. Иймд Löffel abgeben буюу халбагаа үлдээх гэдэг нь насан эцэслэхийг дүрсэлдэг байжээ.</t>
   </si>
   <si>
-    <t>хадан гэртээ харих, нүд аних, амьсгал хураах</t>
+    <t>хадан гэртээ харих; нүд аних; амьсгал хураах</t>
   </si>
   <si>
     <t>Nach langer Krankheit  hat unser Opa mit 95 Jahren den Löffel abgegeben. Er hatte ein glückliches Leben und ist am Ende friedlich eingeschlafen.</t>
@@ -2788,7 +2788,7 @@
     <t>Schock</t>
   </si>
   <si>
-    <t>ам ангайх, алмайран гайхшрах, ам нь эвлэж ядах</t>
+    <t>ам ангайх; алмайран гайхшрах; ам нь эвлэж ядах</t>
   </si>
   <si>
     <t>Bei dem tollen Ausblick bleibt mir die Luft weg.</t>
@@ -2821,7 +2821,7 @@
     <t>Шалгалт, албан ярилцлагын өмнө мэдрэгддэг айдас, түгшүүрийг хэлнэ.</t>
   </si>
   <si>
-    <t>үстэй толгой арзайх, зүрх амаар гарах, зүрх үхэх, баас алдах, чацгаа хавчих, шээс алдах, Muffensausen kriegen / haben, Aftersausen kriegen / bekommen</t>
+    <t>үстэй толгой арзайх; зүрх амаар гарах; зүрх үхэх; баас алдах; чацгаа хавчих; шээс алдах; Muffensausen kriegen / haben; Aftersausen kriegen / bekommen</t>
   </si>
   <si>
     <t>Ich habe echt Muffensausen vor der Präsentation.</t>
@@ -2857,10 +2857,10 @@
     <t>Bewertung</t>
   </si>
   <si>
-    <t>сүр болгох, сүр бадруулах, өчүүхэн зүйлийг уул чинээ болгох</t>
-  </si>
-  <si>
-    <t>Das ist doch nur ein kleiner Kratzer – mach doch nicht aus einer Mücke einen Elefanten!</t>
+    <t>сүр болгох; сүр бадруулах; өчүүхэн зүйлийг уул чинээ болгох</t>
+  </si>
+  <si>
+    <t>Das ist doch nur ein kleiner Kratzer – mach nicht aus einer Mücke einen Elefanten!</t>
   </si>
   <si>
     <t>Bei ihr ist immer Drama. Sie macht aus jeder Mücke einen Elefanten.</t>
@@ -2875,7 +2875,7 @@
     <t>Er neigt dazu, Situationen zu übertreiben und aus einer Mücke einen Elefanten zu machen.</t>
   </si>
   <si>
-    <t xml:space="preserve">aus einer; Mücke einen Elefanten; machen; mach; macht; aus jeder; </t>
+    <t>macht aus jeder Mücke einen Elefanten; aus einer Mücke einen Elefanten machen; aus einer Mücke einen Elefanten zu machen; mach nicht aus einer Mücke einen Elefanten;</t>
   </si>
   <si>
     <t>ph00082</t>
@@ -2890,7 +2890,7 @@
     <t>Vertraulichkeit</t>
   </si>
   <si>
-    <t>хуучлах, дотроо уудлах, нууцаа задлах, ам алдах</t>
+    <t>хуучлах, дотроо уудлах; нууцаа задлах, ам алдах</t>
   </si>
   <si>
     <t>Nach ein paar Drinks fing unser Chef an, aus dem Nähkästchen zu plaudern und hat einige Geheimnisse über die Firma erzählt.</t>
@@ -2926,7 +2926,7 @@
     <t>Үргэлж төгс өнгөрсөн цагт (Perfekt) хэрэглэнэ.</t>
   </si>
   <si>
-    <t>ухаангүй дурлах, донттолоо сонирхох</t>
+    <t>ухаангүй дурлах; донттолоо сонирхох</t>
   </si>
   <si>
     <t>Warum hast du so einen Narren an diesem langweiligen Spiel gefressen?</t>
@@ -2941,7 +2941,7 @@
     <t>Sie ist vernarrt in ihren neuen Hund und redet nur noch von ihm.</t>
   </si>
   <si>
-    <t>einen Narren; an; gefressen; haben; hast; hat; ist vernarrt in; vernarrt in jmdn. / etw. sein;</t>
+    <t>vernarrt in; einen Narren an; gefressen; haben; hast; hat; etw. sein; jmdn.; ist;</t>
   </si>
   <si>
     <t>ph00084</t>
@@ -2992,7 +2992,7 @@
     <t>Энэхүү хэлц нь 20-р зуунд тулааны спортын хэллэгээс үүссэн бөгөөд анх “цохилт даах чадвартай байх” гэсэн утгатай байжээ. Хожим нь энэ утга нь өргөжиж сэтгэл санааны болон бие махбодын сорилтыг тэсэх чадвартай байх гэсэн утгаар хэрэглэгдэх болсон.</t>
   </si>
   <si>
-    <t>сэтгэлийн хаттай байх, зовлон даадаг</t>
+    <t>сэтгэлийн хаттай байх; зовлон даадаг</t>
   </si>
   <si>
     <t>Keine Sorge, ich bin hart im Nehmen. Zur Not arbeite ich die ganze Nacht.</t>
@@ -3130,7 +3130,7 @@
     <t xml:space="preserve">Сармагчин аюул мэдэрсэн үедээ модруу авирч, дээрээс хашхиран өөрийгөө хамгаалдаг үйлдэлтэй зүйрлэн бүтжээ. </t>
   </si>
   <si>
-    <t>тэвчээр алдуулах, галзуурах шахах</t>
+    <t>тэвчээр алдуулах; галзуурах шахах</t>
   </si>
   <si>
     <t>Seine dummen Worte bringen mich auf die Palme!</t>
@@ -3202,7 +3202,7 @@
     <t>Keine zehn Pferde bringen ihn dazu, seine Meinung zu ändern.</t>
   </si>
   <si>
-    <t>Obwohl alle sie überreden wollten, blieb sie standhaft. Keine zehn Pferde hätten sie zum Umzug bewegen können.</t>
+    <t>Obwohl alle sie überreden wollten, blieb sie standhaft. Keine zehn Pferde hätten sie zu diesem Schritt bewegen können.</t>
   </si>
   <si>
     <t>Mich bringen keine zehn Pferde dazu, so früh aufzustehen.</t>
@@ -3211,7 +3211,7 @@
     <t>Er ist so stur, dass keine zehn Pferde ihn von seiner Meinung abbringen können.</t>
   </si>
   <si>
-    <t>bringen; keine zehn Pferde; dazu; zu; abbringen; bewegen;</t>
+    <t>bringen; keine zehn Pferde; dazu; zu ; abbringen; bewegen;</t>
   </si>
   <si>
     <t>ph00092</t>
@@ -3229,7 +3229,7 @@
     <t>Unsinn</t>
   </si>
   <si>
-    <t>бурах, үлгэр шиг юм ярих</t>
+    <t>бурах; үлгэр шиг юм ярих</t>
   </si>
   <si>
     <t>Erzähl mir keinen vom Pferd! Das glaubst du doch selbst nicht!</t>
@@ -3265,7 +3265,7 @@
     <t>Шүүмж, сөрөг үнэлэмж, урам хугарсан утга илэрхийлнэ.</t>
   </si>
   <si>
-    <t>нуухыг нь авах гээд нүдийг нь сохлох, их санасан газар есөн шөнө хоосон</t>
+    <t>нуухыг нь авах гээд нүдийг нь сохлох; их санасан газар есөн шөнө хоосон</t>
   </si>
   <si>
     <t>Sie dachte, sie wäre in der neuen Firma gut aufgehoben, aber sie ist vom Pferd auf den Esel gekommen.</t>
@@ -3526,7 +3526,7 @@
     <t>Энэ хэллэг нь дундад зууны үеийн торх үйлдвэрлэлтэй холбоотой үүссэн байна. Торхыг барьж, тогтоох зориулалттай төмөр цагариг бүслүүр задарвал торх эвдрэнэ. Энэхүү дүрслэл нь хүний төсөөлөлд ямар нэг зүйл тухайн нөхцөл байдлаас шалтгаалан хяналтаас гарч буйг илэрхийлдэг.</t>
   </si>
   <si>
-    <t>хөл хөөрцөг болох, бөөн баяр болох, хөл толгойгоо ал- дах, эх адаггүй болох, außer Rand und Band sein</t>
+    <t>хөл хөөрцөг болох; бөөн баяр болох; хөл толгойгоо алдах; эх адаггүй болох; außer Rand und Band sein</t>
   </si>
   <si>
     <t>Die Kinder geraten oft außer Rand und Band, wenn sie zu viel Zucker essen.</t>
@@ -3556,7 +3556,7 @@
     <t>Belastung</t>
   </si>
   <si>
-    <t>галд тос нэмэх / хийх, сүүлчийн цохилт өгөх</t>
+    <t>галд тос нэмэх / хийх; сүүлчийн цохилт өгөх</t>
   </si>
   <si>
     <t>Die schlechte Nachricht hat ihm endgültig den Rest gegeben.</t>
@@ -3589,7 +3589,7 @@
     <t>Дундад зууны үеийн туульс, домогт нууцлаг морьтон баатруудын тухай өгүүлдэг байжээ. Эдгээр баатрууд нь хуяг дуулга өмссөн байдаг тул хэн болохыг нь таних боломжгүй байсан. Тэднийг хэн болохыг мэдэх нь нэн чухал байсан учир нэрийг нь чанга дуудан  танилцуулдаг уламжлалаас үүсэлтэй.</t>
   </si>
   <si>
-    <t>нэр усыг нь зарлах, нууж хаалгүй, ний нуугүй хэлэх, Tacheles reden, Klartext sprechen</t>
+    <t>нэр усыг нь зарлах; нууж хаалгүй; ний нуугүй хэлэх; Tacheles reden; Klartext sprechen</t>
   </si>
   <si>
     <t>Jetzt nenn doch endlich Ross und Reiter, wer hat das wirklich gesagt?</t>
@@ -3655,7 +3655,7 @@
     <t>schmoren гэдэг нь махыг шүү- сэнд нь удаан болгохыг хэлнэ. Харин jmdn. im eigenen Saft schmoren lassen нь хэн нэгнийг таагүй байдалд орхих, туслахгүй хаях гэсэн утга илэрхийлнэ.</t>
   </si>
   <si>
-    <t>зовлонтойгоо нүүр тулж шаналах, зовлонгоо үүрэх</t>
+    <t>зовлонтойгоо нүүр тулж шаналах; зовлонгоо үүрэх</t>
   </si>
   <si>
     <t>Wenn du dich ständig ärgerst und niemandem davon erzählst, wirst du am Ende nur im eigenen Saft schmoren.</t>
@@ -3691,7 +3691,7 @@
     <t>Энэхүү хэлцийн гарал тодорхойгүй боловч олон таамаг байдгийн нэг нь дундад зуунд хог ачдаг үйлчилгээ байхгүй байснаас хүмүүс хогоо үүдэндээ гаргаж хаядаг байжээ. Гахайнуудаа хашаанаас нь гаргах үед тэд хог дээр очиж, хогийг нь идэж, бусниулдаг байжээ.</t>
   </si>
   <si>
-    <t>дураараа дургиж, дунд чөмгөөрөө жиргэх, задгай авах, балай авах, хөлөөрөө толгой хийх</t>
+    <t>дураараа дургиж; дунд чөмгөөрөө жиргэх; задгай авах; балай авах; хөлөөрөө толгой хийх</t>
   </si>
   <si>
     <t>Und heute Abend nach der Prüfung lassen wir mal so richtig die Sau raus!</t>
@@ -3724,7 +3724,7 @@
     <t>Энэхүү хэллэг нь дундад зуунд гэмт хэрэгтнүүдийг олон нийтийн өмнө доромжлон, шившиг болгохын тулд тэднийг гахайн толгойн хэлбэртэй төмөр маск зүүлгэн гудамжаар дөрөв хөллөн явуулдаг байжээ.</t>
   </si>
   <si>
-    <t>доромжлох, шив- шиг болгох, зад загинах, доош нь хийх</t>
+    <t>доромжлох; шившиг болгох; зад загинах; доош нь хийх</t>
   </si>
   <si>
     <t>Gestern machte unser Chef das gesamte Team zur Sau – er war wirklich wütend!</t>
@@ -3784,7 +3784,7 @@
     <t>Schimmer нь гэрэл, гялбаа гэсэн утгатай. Хэрвээ blassen Schimmer буюу сүүмэлзэх цайвар гэрэл ч байхгүй бол, тухайн зүйлийн талаар огтхонч ойлголтгүй гэсэн үг.</t>
   </si>
   <si>
-    <t>keine Ahnung haben, nur Bahnhof verstehen, keinen (blassen) Dunst (von etw.) haben</t>
+    <t>keine Ahnung haben; nur Bahnhof verstehen; keinen (blassen) Dunst (von etw.) haben</t>
   </si>
   <si>
     <t>Als Anfänger hat man erst mal keinen Schimmer!</t>
@@ -3814,7 +3814,7 @@
     <t>Тулааны өмнө цэргүүдэд айдсаас үүдэн хоол боловсруулах эрхтэн тогтолцоонд асуудал үүсэхэд энэхүү хэлцээр илэрхийлдэг байсан гэж үздэг.</t>
   </si>
   <si>
-    <t>сүүлээ хавчих,сүнс зайлах, бөгсөө хавчих, зүрх амаар гарах, үнхэлцэг хагарах, vor jmdn. / etw. Schiss kriegen</t>
+    <t>сүүлээ хавчих; сүнс зайлах; бөгсөө хавчих; зүрх амаар гарах; үнхэлцэг хагарах; vor jmdn. / etw. Schiss kriegen</t>
   </si>
   <si>
     <t>Ich habe echt Schiss vor der Prüfung und kann kaum schlafen.</t>
@@ -3886,7 +3886,7 @@
     <t>Бодол ус шиг урсдаг гэсэн санаанаас уг хэллэг үүссэн. Хэрэв усны шланк дээр зогсвол усны урсгалыг хааж, ус урсахаа болихтой зүйрлэжээ.</t>
   </si>
   <si>
-    <t>гацаанд орох, сүлжээ унах</t>
+    <t>гацаанд орох; сүлжээ унах</t>
   </si>
   <si>
     <t>Kannst du mir bei Mathe helfen? Ich stehe total auf dem Schlauch.</t>
@@ -3913,7 +3913,7 @@
     <t>хэн нэгэнд дурлах үед мэдрэгддэг догдлол, баяр хөөрийн мэдрэмж</t>
   </si>
   <si>
-    <t>барьц алдах, балмагдах, догдлох</t>
+    <t>барьц алдах; балмагдах; догдлох</t>
   </si>
   <si>
     <t>Jedes Mal, wenn ich ihn sehe, habe ich Schmetterlinge im Bauch.</t>
@@ -3946,7 +3946,7 @@
     <t>kalter Kaffee ижил утгатай. olle Kamellen сонирхолтой биш, хүн болгоны мэддэг зүйлийг дахин дахин ярихад дургүйцлээ илэрхийлэх үед хэрэглэнэ.</t>
   </si>
   <si>
-    <t>үлэг болсон юм ярих, дэвэн галавын юм ярих</t>
+    <t>үлэг болсон юм ярих; дэвэн галавын юм ярих</t>
   </si>
   <si>
     <t>Das ist doch Schnee von gestern!</t>
@@ -4021,7 +4021,7 @@
     <t>Сайн таньдаг, дотны хүмүүсийн хүрээнд хэн нэгэнд санаа зовон өөрт нь хандаж хэлэх эсвэл санаа зовж буй өөр хэн нэгний талаар ярихад хэрэглэнэ. Мөн хэлж байгаа дууны өнгөөс хамаарч дооглонгүй утга илэрхийлж болно.</t>
   </si>
   <si>
-    <t>хөөрхий амьтан, золгүй амьтан, аз нь харьсан амьтан / хүн</t>
+    <t>хөөрхий амьтан; золгүй амьтан; аз нь харьсан амьтан / хүн</t>
   </si>
   <si>
     <t>Du armes Schwein, du musstest das ganze Wochenende durcharbeiten und jetzt bist du total erschöpft.</t>
@@ -4091,7 +4091,7 @@
     <t>Энэхүү хэлцийн гарал тодорхойгүй боловч олон таамаг байдгийн нэг нь дээр үед германд Schützenfeste буюу анчдын баяраар хамгийн муу буудсан  анчныг урамшуулан гахайгаар шагнадаг байжээ. Мөн дундад зуунд одоогийн хөзрийн тамга Sau буюу “мэгж” нэртэй байсан бөгөөд энэ хөзрийг авсан хүн ялах магадлал их байв.</t>
   </si>
   <si>
-    <t>аз ивээх, аз дай- рах, тэнгэрийн умдаг атгах</t>
+    <t>аз ивээх; аз дайрах; тэнгэрийн умдаг атгах</t>
   </si>
   <si>
     <t>Schwein muss man haben, wenn man bei der Lotterie gewinnt.</t>
@@ -4127,7 +4127,7 @@
     <t>Биеэ зохисгүй авч явах, бүдүүлэг гэсэн утгаас гадна хүн чанаргүй, зохисгүй, ёс зүйгүй, болчимгүй зан гаргахыг хэлнэ</t>
   </si>
   <si>
-    <t xml:space="preserve">гахай нохой шиг, хүний мөсгүй </t>
+    <t xml:space="preserve">гахай нохой шиг; хүний мөсгүй </t>
   </si>
   <si>
     <t>Michael hat keine Manieren, er hat sich im Restaurant wie ein Schwein benommen.</t>
@@ -4157,7 +4157,7 @@
     <t>seelischer Schmerz</t>
   </si>
   <si>
-    <t>сэтгэл  өвдөх, сэт- гэл эмтрэх, элэг эмтрэх, зүрх шимшрэх, элэг эгших</t>
+    <t>сэтгэл  өвдөх; сэтгэл эмтрэх; элэг эмтрэх; зүрх шимшрэх; элэг эгших</t>
   </si>
   <si>
     <t>Wenn ich jemanden sehe, der auf der Straße lebt, tut mir das in der Seele weh.</t>
@@ -4226,7 +4226,7 @@
     <t>Энэ хэллэг нь театрын уран бүтээлээс гаралтай бөгөөд тухайн хүний үйлдлийг тайзны үзүүлбэртэй зүйрлэж, хэт их драматик байдлыг илэрхийлдэг.</t>
   </si>
   <si>
-    <t>сүржигнэх, сүр бадруулах, Theater machen</t>
+    <t>сүржигнэх; сүр бадруулах; Theater machen</t>
   </si>
   <si>
     <t>Als mein Kollege spät kam, hat seine Frau ihm vor allen Leuten eine Szene gemacht.</t>
@@ -4256,7 +4256,7 @@
     <t>Tacheles буюу зорилго, гол асуудал гэх еврей үгнээс гаралтай.</t>
   </si>
   <si>
-    <t>ам нээвэл уушиг нээх, шулуухан ярих</t>
+    <t>ам нээвэл уушиг нээх; шулуухан ярих</t>
   </si>
   <si>
     <t>Ich muss dir endlich die Wahrheit sagen, was ich davon halte. Wir müssen Tacheles reden. Sonst kommen wir keinen Schritt weiter.</t>
@@ -4286,7 +4286,7 @@
     <t>eine Macke haben, einen Dachschaden haben, eine Schraube locker haben, nicht alle Latten am Zaun haben, nicht ganz dicht sein адил утгатай хэрэглэнэ.</t>
   </si>
   <si>
-    <t>толгойдоо юмтай, эрэг шураг нь дутуу</t>
+    <t>толгойдоо юмтай; эрэг шураг нь дутуу</t>
   </si>
   <si>
     <t>Er sagt, er möchte im Park Picknick machen – aber es regnet doch! Er hat nicht alle Tassen im Schrank!</t>
@@ -4313,7 +4313,7 @@
     <t>Perspektivwechsel</t>
   </si>
   <si>
-    <t>хайрцагнаас гарч сэтгэх, задгай сэтгэх, über den Tellerrand blicken</t>
+    <t>хайрцагнаас гарч сэтгэх; задгай сэтгэх; über den Tellerrand blicken</t>
   </si>
   <si>
     <t>Es ist wichtig, über den Tellerrand zu schauen und andere Kulturen kennenzulernen.</t>
@@ -4349,7 +4349,7 @@
     <t>Христийн шашнаас гаралтай бөгөөд чөтгөр гэрт нь орохоос сэргийлж хаалганы дээр тэмдэг зурдаг байснаас үүдэлтэй.  Харин чөтгөр зурвал муу зүйлсийг дуудна гэж үздэг байжээ.</t>
   </si>
   <si>
-    <t>муу ёрлох, муу амлах</t>
+    <t>муу ёрлох; муу амлах</t>
   </si>
   <si>
     <t>Ich habe geträumt, dass ich meinen Ring verloren habe. – Das ist nur ein Traum gewesen, male nicht direkt den Teufel an die Wand.</t>
@@ -4361,7 +4361,7 @@
     <t>Ich will den Teufel nicht an die Wand malen, aber was ist, wenn du die Prüfung nicht schaffst?</t>
   </si>
   <si>
-    <t xml:space="preserve">den Teufel an die Wand; malen; male; malst; </t>
+    <t xml:space="preserve">den Teufel; an die Wand; malen; male; malst; </t>
   </si>
   <si>
     <t>ph00127</t>
@@ -4442,7 +4442,7 @@
     <t>Эрт үед сэтгэцийн өвчтэй хүний толгойд шувуу үүрлэж, оюун ухааныг нь хэвийн бус болгодог гэж үздэг байжээ.</t>
   </si>
   <si>
-    <t>юмтай байх, bei dir piept’s wohl</t>
+    <t>юмтай байх; bei dir piept’s wohl</t>
   </si>
   <si>
     <t>Als er mir diese Geschichte erzählte, musste ich ihm wirklich einen Vogel zeigen, so unglaubwürdig klang das.</t>
@@ -4478,7 +4478,7 @@
     <t xml:space="preserve">Waffel гэдэг нь энэ хэлцэд идэх юм биш харин том амтай гэсэн утгаар хэрэглэгдэнэ. waffeln буюу schwafeln нь дэмий балай, утгагүй юм ярих гэсэн утгатай. Англи хэлний waffle үйл үгтэй утгын хувьд төстэй. </t>
   </si>
   <si>
-    <t>галзуу, солиотой юм шиг</t>
+    <t>галзуу; солиотой юм шиг</t>
   </si>
   <si>
     <t>Hast du einen an der Waffel, oder warum ziehst du jetzt schon wieder um?</t>
@@ -4508,7 +4508,7 @@
     <t>Krise</t>
   </si>
   <si>
-    <t>хоолой дээр тулах, амь наана, там цаана, das Wasser bis zum Hals stehen</t>
+    <t>хоолой дээр тулах, амь наана; там цаана; das Wasser bis zum Hals stehen</t>
   </si>
   <si>
     <t>Ich kann den Kredit nicht mehr bezahlen – mir steht das Wasser bis zum Hals.</t>
@@ -4571,7 +4571,7 @@
     <t>Ихэвчлэн сэтгэл хөдлөлдөө амархан автаж, кино, ном гэх мэт сэтгэл хөдөлгөсөн үйл явдлын үеэр амархан уйлдаг хүмүүсийг дүрслэхэд хэрэглэнэ. Заримдаа шог, эсвэл өхөөрдөж хэлэх тохиолдол байдагч доромж байдлаар ашигладаггүй. Heulsuse гэвэл уйланхай хүнийг дургүйцсэн эсвэл дооглосон маягаар хэлж болно.</t>
   </si>
   <si>
-    <t>усан нүдлэх, нулимс ойрхон байх</t>
+    <t>усан нүдлэх; нулимс ойрхон байх</t>
   </si>
   <si>
     <t>Weinen im Kino ist normal für mich – ich bin echt nah am Wasser gebaut.</t>
@@ -4598,7 +4598,7 @@
     <t>Энэ хэлц үг нь дарханы ажлаас гаралтай. Төмрийг олон үе шаттайгаар хайлуулж, хэвэнд цутгадаг бөгөөд төмөр хамгийн өндөр халалтын түвшинд хүрэхэд Weißglut буюу цагаан өнгийн цог үүсдэг байна. Хүний уурыг туйлд нь хүргэхийг энэхүү зүйрлэлээр дүрсэлжээ.</t>
   </si>
   <si>
-    <t>цус харвуулах шахах, тэсрэхэд хүргэх, jmdn. (bis) zur Weißglut reizen</t>
+    <t>цус харвуулах шахах; тэсрэхэд хүргэх; jmdn. (bis) zur Weißglut reizen</t>
   </si>
   <si>
     <t>Seine Faulheit hat sie zur Weißglut gebracht.</t>
@@ -4628,7 +4628,7 @@
     <t xml:space="preserve">Ихэвчлэн аз жаргал, хайр болон амжилттай холбоотой сэдвийн хүрээнд хэрэглэгддэг. Жишээ нь: гэрлэх санал тавих, ажлын ярилцлагад тэнцэх гэх мэт үед ашигладаг. </t>
   </si>
   <si>
-    <t>хагартлаа баярлах, магнай хагартал баярлах, сайхан ааш хөдлөх, хөл газар хүрэхгүй баярлах, die ganze Welt umarmen mögen</t>
+    <t>хагартлаа баярлах; магнай хагартал баярлах; сайхан ааш хөдлөх; хөл газар хүрэхгүй баярлах; die ganze Welt umarmen mögen</t>
   </si>
   <si>
     <t>Nach der bestandenen Prüfung wollte sie die ganze Welt umarmen.</t>
@@ -4655,7 +4655,7 @@
     <t>Trennung</t>
   </si>
   <si>
-    <t>jmdn. den Laufpass geben; jmdn. abservieren; jmdn. fallen lassen; хөсөр хаях; хог дээр хаях; жийх</t>
+    <t>хөсөр хаях; хог дээр хаях; жийх; jmdn. den Laufpass geben; jmdn. abservieren; jmdn. fallen lassen;</t>
   </si>
   <si>
     <t>Nach drei Jahren Beziehung hat sie ihn einfach in den Wind geschossen.</t>
@@ -4691,7 +4691,7 @@
     <t>Найз нөхдийн хүрээнд, ихэвчлэн хөгжилтэй байдлаар хэрэглэх хэллэг. Утга нь зүгээр нэг их алхах биш, бүр ер бусын их алхсныг илтгэнэ.</t>
   </si>
   <si>
-    <t>sich die Füße wundlaufen, sich die Hacken ablaufen, тавхайгаа эргэтэл алхах, үхтлээ алхах</t>
+    <t>тавхайгаа эргэтэл алхах; үхтлээ алхах; sich die Füße wundlaufen; sich die Hacken ablaufen</t>
   </si>
   <si>
     <t>Einmal durch ganz Berlin zu Fuß? - Da läuft man sich ja einen Wolf!</t>
@@ -4769,7 +4769,7 @@
     <t>Fleischwolf гэдэг нь “махны машин” гэсэн утгатай бөгөөд маш их ядарч туйлдсан байгаа хүнийг “махны машинд хийгээд эргүүлчихсэн юм шиг” гэж зүйрлэжээ.</t>
   </si>
   <si>
-    <t>царай алдах, салж унах, гундах, sich fühlen wie durch den Fleischwolf gedreht</t>
+    <t>царай алдах; салж унах; гундах; sich fühlen wie durch den Fleischwolf gedreht</t>
   </si>
   <si>
     <t>Wenn ich am Freitagabend nach Hause komme, fühle ich mich wie durch den Wolf gedreht.</t>
@@ -4790,7 +4790,7 @@
     <t>маш их аз жаргалтай байх, баяр хөөрөөр дүүрэн байх, дурласан байх</t>
   </si>
   <si>
-    <t>нар нь гарах, хөл нь газар хүрэхгүй баярлах, үүлэн дээр хөвөх, auf Wolke sieben schweben</t>
+    <t>нар нь гарах; хөл нь газар хүрэхгүй баярлах; үүлэн дээр хөвөх; auf Wolke sieben schweben</t>
   </si>
   <si>
     <t>Seitdem sie verliebt ist, schwebt sie auf Wolke sieben.</t>
@@ -4826,7 +4826,7 @@
     <t>Бөс даавууг будганд оруулаад өлгөхөд ногоон эсвэл шар өнгөтэй байсан даавуу хүчилтөрөгчтэй химийн урвалд орж цэнхэр болж хувирсан нь хүмүүсийг балмагдуулсан тул энэхүү хэлц үүссэн гэдэг.</t>
   </si>
   <si>
-    <t>auf die Nase fallen, die Quittung bekommen</t>
+    <t>auf die Nase fallen; die Quittung bekommen</t>
   </si>
   <si>
     <t>Wenn du nichts lernst, wirst du in der Prüfung ein blaues Wunder erleben!</t>
@@ -4859,7 +4859,7 @@
     <t>sich für jmdn. ins Zeug legen гэвэл хэн нэгний төлөө ямар нэг зүйлийг бүх хүчээ шавхан хийх, туслах гэсэн утга илэрхийлнэ.</t>
   </si>
   <si>
-    <t>хөлсөө дуслуулах, морь нохой мэт зүтгэх, sich für jmdn./etw. (schwer / mächtig) ins Zeug werfen</t>
+    <t>хөлсөө дуслуулах; морь нохой мэт зүтгэх; sich für jmdn./etw. (schwer / mächtig) ins Zeug werfen</t>
   </si>
   <si>
     <t>Um das Projekt rechtzeitig abzuschließen, musste sie sich richtig ins Zeug legen.</t>
@@ -4926,8 +4926,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor rgb="FFF4CCCC"/>
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -4959,7 +4959,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -6207,7 +6207,7 @@
       <c r="AE15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="7" t="s">
         <v>196</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -7206,7 +7206,7 @@
       <c r="AE30" s="2"/>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="7" t="s">
         <v>375</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -7404,7 +7404,7 @@
       <c r="A34" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="7" t="s">
         <v>407</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -7797,7 +7797,7 @@
       <c r="AE39" s="2"/>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="7" t="s">
         <v>477</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -8387,7 +8387,7 @@
       <c r="A49" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="7" t="s">
         <v>579</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -9367,7 +9367,7 @@
       <c r="AE63" s="2"/>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="7" t="s">
         <v>745</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -9762,7 +9762,7 @@
       <c r="A70" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="7" t="s">
         <v>810</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -9829,7 +9829,7 @@
       <c r="A71" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="7" t="s">
         <v>820</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -9893,7 +9893,7 @@
       <c r="AE71" s="2"/>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="7" t="s">
         <v>831</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -10303,7 +10303,7 @@
       <c r="F78" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G78" s="7" t="s">
+      <c r="G78" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H78" s="1" t="s">
@@ -10422,7 +10422,7 @@
       <c r="A80" s="1" t="s">
         <v>913</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="7" t="s">
         <v>914</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -10689,7 +10689,7 @@
       <c r="AE83" s="2"/>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="7" t="s">
         <v>958</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -11152,7 +11152,7 @@
       <c r="AE90" s="2"/>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="7" t="s">
         <v>1036</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -11284,7 +11284,7 @@
       <c r="AE92" s="2"/>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="7" t="s">
         <v>1058</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -12271,7 +12271,7 @@
       <c r="AE107" s="2"/>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="s">
+      <c r="A108" s="7" t="s">
         <v>1223</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -12404,7 +12404,7 @@
       <c r="A110" s="1" t="s">
         <v>1243</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="7" t="s">
         <v>1244</v>
       </c>
       <c r="C110" s="1" t="s">
@@ -13470,7 +13470,7 @@
       <c r="A126" s="1" t="s">
         <v>1419</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" s="7" t="s">
         <v>1420</v>
       </c>
       <c r="C126" s="1" t="s">
@@ -14125,7 +14125,7 @@
       <c r="AE135" s="2"/>
     </row>
     <row r="136">
-      <c r="A136" s="1" t="s">
+      <c r="A136" s="7" t="s">
         <v>1523</v>
       </c>
       <c r="B136" s="1" t="s">

</xml_diff>